<commit_message>
act dbs excell 11022020
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/MODELOS.xlsx
+++ b/EXCEL LIBS/MODELOS.xlsx
@@ -4417,9 +4417,6 @@
     <t>ODENSLUNDA</t>
   </si>
   <si>
-    <t>Categorias Produto : 04-02-2020 15:43:05</t>
-  </si>
-  <si>
     <t>1062</t>
   </si>
   <si>
@@ -4436,6 +4433,9 @@
   </si>
   <si>
     <t>KLIPPAN LVL</t>
+  </si>
+  <si>
+    <t>Categorias Produto : 11-02-2020 10:32:08</t>
   </si>
 </sst>
 </file>
@@ -4846,8 +4846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G741"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A595" workbookViewId="0">
-      <selection activeCell="G692" sqref="G692"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4874,7 +4874,7 @@
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>1464</v>
+        <v>1470</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -7070,10 +7070,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B98" s="5" t="s">
         <v>1465</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>1466</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>10</v>
@@ -7116,10 +7116,10 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>1467</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>1468</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>10</v>
@@ -7139,10 +7139,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B101" s="5" t="s">
         <v>1469</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>1470</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
act db excell 26022020
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/MODELOS.xlsx
+++ b/EXCEL LIBS/MODELOS.xlsx
@@ -4435,13 +4435,13 @@
     <t>KLIPPAN LVL</t>
   </si>
   <si>
-    <t>Categorias Produto : 21-02-2020 11:18:07</t>
-  </si>
-  <si>
     <t>1080</t>
   </si>
   <si>
     <t>CHACAL</t>
+  </si>
+  <si>
+    <t>Categorias Produto : 26-02-2020 09:05:59</t>
   </si>
 </sst>
 </file>
@@ -4880,7 +4880,7 @@
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>1470</v>
+        <v>1472</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -7191,10 +7191,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>1471</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>1472</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>10</v>

</xml_diff>